<commit_message>
improv methods for CWS analysis
</commit_message>
<xml_diff>
--- a/src/nlp/data/tag_keywords_lists.xlsx
+++ b/src/nlp/data/tag_keywords_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandd/projects/sr2ml/src/nlp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9200997D-3CAF-BD4C-B760-7C5049D67FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3E766-D004-9D4A-B6FF-8929B823E0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20700" activeTab="7" xr2:uid="{97522036-D9BC-AD48-9993-E39060B5165E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" activeTab="4" xr2:uid="{97522036-D9BC-AD48-9993-E39060B5165E}"/>
   </bookViews>
   <sheets>
     <sheet name="comp_mech" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="2344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="2343">
   <si>
     <t>welded joint</t>
   </si>
@@ -6192,12 +6192,6 @@
     <t>cutting</t>
   </si>
   <si>
-    <t>cleaning</t>
-  </si>
-  <si>
-    <t>plating</t>
-  </si>
-  <si>
     <t>brushing</t>
   </si>
   <si>
@@ -6222,12 +6216,6 @@
     <t>heat-treating</t>
   </si>
   <si>
-    <t>repairing</t>
-  </si>
-  <si>
-    <t>refurbishing</t>
-  </si>
-  <si>
     <t>Hot Blackening</t>
   </si>
   <si>
@@ -6717,9 +6705,6 @@
     <t>lubrication</t>
   </si>
   <si>
-    <t>repackaging</t>
-  </si>
-  <si>
     <t>installation</t>
   </si>
   <si>
@@ -7075,6 +7060,18 @@
   </si>
   <si>
     <t xml:space="preserve">Solid state </t>
+  </si>
+  <si>
+    <t>repack</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>refurbish</t>
+  </si>
+  <si>
+    <t>clean</t>
   </si>
 </sst>
 </file>
@@ -7518,16 +7515,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>2142</v>
+        <v>2138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>2141</v>
+        <v>2137</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>2143</v>
+        <v>2139</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -7722,7 +7719,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>2177</v>
+        <v>2173</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>247</v>
@@ -7815,7 +7812,7 @@
         <v>1682</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>2195</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -8005,7 +8002,7 @@
         <v>101</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>2192</v>
+        <v>2188</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>1691</v>
@@ -8117,7 +8114,7 @@
         <v>193</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>2194</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
@@ -8170,7 +8167,7 @@
         <v>249</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>2193</v>
+        <v>2189</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>1708</v>
@@ -8181,7 +8178,7 @@
         <v>313</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>2191</v>
+        <v>2187</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>212</v>
@@ -8616,7 +8613,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="4" t="s">
-        <v>2189</v>
+        <v>2185</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>231</v>
@@ -8690,7 +8687,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" s="4" t="s">
-        <v>2238</v>
+        <v>2233</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>97</v>
@@ -8834,7 +8831,7 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A123" s="4" t="s">
-        <v>2178</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
@@ -8889,7 +8886,7 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A134" s="4" t="s">
-        <v>2196</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.15">
@@ -8944,7 +8941,7 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A145" s="4" t="s">
-        <v>2190</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.15">
@@ -8974,7 +8971,7 @@
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A151" s="4" t="s">
-        <v>2197</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.15">
@@ -9104,7 +9101,7 @@
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="s">
-        <v>2198</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.15">
@@ -9164,7 +9161,7 @@
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
-        <v>2239</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.15">
@@ -9223,10 +9220,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>2145</v>
+        <v>2141</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2146</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -9656,12 +9653,12 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
-        <v>2186</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
-        <v>2188</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
@@ -9681,7 +9678,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="s">
-        <v>2201</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
@@ -9901,7 +9898,7 @@
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A124" s="4" t="s">
-        <v>2170</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
@@ -10341,7 +10338,7 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>2200</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.15">
@@ -10401,7 +10398,7 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>2169</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.15">
@@ -10541,7 +10538,7 @@
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="s">
-        <v>2199</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.15">
@@ -10606,7 +10603,7 @@
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="s">
-        <v>2187</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.15">
@@ -10751,7 +10748,7 @@
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="s">
-        <v>2185</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.15">
@@ -10816,7 +10813,7 @@
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="s">
-        <v>2168</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.15">
@@ -10861,7 +10858,7 @@
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="s">
-        <v>2167</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.15">
@@ -11229,22 +11226,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2146</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2147</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>2148</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2149</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2150</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2151</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2152</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -11284,7 +11281,7 @@
         <v>303</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>2216</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -11438,7 +11435,7 @@
         <v>1038</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>2276</v>
+        <v>2271</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>446</v>
@@ -11461,7 +11458,7 @@
         <v>351</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>2215</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -11472,7 +11469,7 @@
         <v>988</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>2277</v>
+        <v>2272</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>450</v>
@@ -11567,7 +11564,7 @@
         <v>318</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>2203</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.15">
@@ -11578,7 +11575,7 @@
         <v>409</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>2204</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.15">
@@ -11600,7 +11597,7 @@
         <v>319</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>2205</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.15">
@@ -11677,7 +11674,7 @@
         <v>1020</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>2206</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="16" x14ac:dyDescent="0.2">
@@ -11795,7 +11792,7 @@
         <v>954</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>2207</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.15">
@@ -11803,7 +11800,7 @@
         <v>416</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>2208</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.15">
@@ -11811,7 +11808,7 @@
         <v>1053</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>2209</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.15">
@@ -11819,7 +11816,7 @@
         <v>335</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>2210</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.15">
@@ -11827,7 +11824,7 @@
         <v>1019</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>2211</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.15">
@@ -11963,7 +11960,7 @@
         <v>1018</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>2212</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.15">
@@ -11987,7 +11984,7 @@
         <v>1040</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>2213</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.15">
@@ -12083,7 +12080,7 @@
         <v>1017</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>2214</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.15">
@@ -12210,7 +12207,7 @@
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C103" s="4" t="s">
-        <v>2202</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.15">
@@ -12249,10 +12246,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>2153</v>
+        <v>2149</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2154</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -12308,7 +12305,7 @@
         <v>1635</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2166</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -12454,7 +12451,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>2217</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -12644,9 +12641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1502DAD1-7392-8F4F-91D6-E58A00062B27}">
   <dimension ref="A1:B227"/>
   <sheetViews>
-    <sheetView zoomScale="182" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -12658,10 +12655,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>2155</v>
+        <v>2151</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2156</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -12714,7 +12711,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>2134</v>
+        <v>2130</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2008</v>
@@ -12754,7 +12751,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>2129</v>
+        <v>2125</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>2047</v>
@@ -12762,7 +12759,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>2133</v>
+        <v>2129</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>2048</v>
@@ -12770,10 +12767,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>2130</v>
+        <v>2126</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>2059</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
@@ -12781,15 +12778,15 @@
         <v>2024</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>2060</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>2049</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -12797,20 +12794,20 @@
         <v>2043</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>2050</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>2135</v>
+        <v>2131</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B20" s="4" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
@@ -12818,7 +12815,7 @@
         <v>349</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
@@ -12826,7 +12823,7 @@
         <v>1967</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
@@ -12834,7 +12831,7 @@
         <v>1933</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
@@ -12842,7 +12839,7 @@
         <v>2039</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
@@ -12850,7 +12847,7 @@
         <v>1978</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
@@ -12858,7 +12855,7 @@
         <v>1932</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
@@ -12874,23 +12871,23 @@
         <v>1984</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>2061</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>2136</v>
+        <v>2132</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>2062</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>2137</v>
+        <v>2133</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>2063</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
@@ -12898,12 +12895,12 @@
         <v>1931</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>2064</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B32" s="4" t="s">
-        <v>2065</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
@@ -12911,7 +12908,7 @@
         <v>1873</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>2066</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
@@ -12919,15 +12916,15 @@
         <v>1995</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>2067</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>2131</v>
+        <v>2127</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>2068</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
@@ -12935,15 +12932,15 @@
         <v>1966</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>2069</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>2138</v>
+        <v>2134</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>2070</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
@@ -12951,7 +12948,7 @@
         <v>1913</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>2071</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
@@ -12959,7 +12956,7 @@
         <v>1937</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>2072</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
@@ -12967,7 +12964,7 @@
         <v>1918</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>2073</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
@@ -12975,15 +12972,15 @@
         <v>1934</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>2074</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>2139</v>
+        <v>2135</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>2075</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
@@ -12991,7 +12988,7 @@
         <v>1955</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>2076</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
@@ -12999,7 +12996,7 @@
         <v>1880</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>2077</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
@@ -13007,12 +13004,12 @@
         <v>2015</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>2078</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B46" s="4" t="s">
-        <v>2079</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
@@ -13020,15 +13017,15 @@
         <v>1883</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>2081</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>2218</v>
+        <v>2214</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>2082</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
@@ -13036,7 +13033,7 @@
         <v>1960</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>2083</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
@@ -13044,15 +13041,15 @@
         <v>1991</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>2084</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>2140</v>
+        <v>2136</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>2085</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
@@ -13060,7 +13057,7 @@
         <v>1872</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>2086</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
@@ -13068,7 +13065,7 @@
         <v>2032</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>2087</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
@@ -13076,7 +13073,7 @@
         <v>2035</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>2088</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.15">
@@ -13084,7 +13081,7 @@
         <v>1865</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>2089</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.15">
@@ -13092,7 +13089,7 @@
         <v>1864</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>2090</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.15">
@@ -13100,7 +13097,7 @@
         <v>1992</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>2091</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.15">
@@ -13108,7 +13105,7 @@
         <v>1874</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>2092</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.15">
@@ -13116,7 +13113,7 @@
         <v>1907</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>2093</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.15">
@@ -13124,7 +13121,7 @@
         <v>1908</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>2094</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.15">
@@ -13132,7 +13129,7 @@
         <v>1877</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>2095</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.15">
@@ -13140,7 +13137,7 @@
         <v>937</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>2096</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.15">
@@ -13148,7 +13145,7 @@
         <v>1917</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>2097</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
@@ -13156,7 +13153,7 @@
         <v>1959</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>2098</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.15">
@@ -13164,7 +13161,7 @@
         <v>1977</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>2099</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">
@@ -13172,7 +13169,7 @@
         <v>1985</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.15">
@@ -13180,7 +13177,7 @@
         <v>2040</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.15">
@@ -13188,7 +13185,7 @@
         <v>1938</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.15">
@@ -13196,7 +13193,7 @@
         <v>1878</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>2103</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.15">
@@ -13204,7 +13201,7 @@
         <v>2045</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>2104</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.15">
@@ -13212,7 +13209,7 @@
         <v>1884</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.15">
@@ -13220,7 +13217,7 @@
         <v>1920</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>2106</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.15">
@@ -13228,7 +13225,7 @@
         <v>1892</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>2107</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.15">
@@ -13236,7 +13233,7 @@
         <v>1993</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>2108</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.15">
@@ -13244,7 +13241,7 @@
         <v>1936</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>2109</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.15">
@@ -13252,7 +13249,7 @@
         <v>1852</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>2110</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.15">
@@ -13260,7 +13257,7 @@
         <v>2021</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>2111</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.15">
@@ -13268,7 +13265,7 @@
         <v>1986</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>2112</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.15">
@@ -13276,7 +13273,7 @@
         <v>1988</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.15">
@@ -13284,7 +13281,7 @@
         <v>1975</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>2114</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.15">
@@ -13292,7 +13289,7 @@
         <v>1922</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>2080</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.15">
@@ -13300,7 +13297,7 @@
         <v>1921</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>2115</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.15">
@@ -13308,7 +13305,7 @@
         <v>2026</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>2094</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.15">
@@ -13316,7 +13313,7 @@
         <v>1886</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>2116</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.15">
@@ -13324,7 +13321,7 @@
         <v>1896</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>2117</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.15">
@@ -13332,7 +13329,7 @@
         <v>1973</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>2118</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.15">
@@ -13340,7 +13337,7 @@
         <v>1974</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>2119</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.15">
@@ -13348,7 +13345,7 @@
         <v>1891</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.15">
@@ -13356,7 +13353,7 @@
         <v>1862</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>2121</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.15">
@@ -13364,7 +13361,7 @@
         <v>1863</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.15">
@@ -13372,7 +13369,7 @@
         <v>2027</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>2103</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.15">
@@ -13380,7 +13377,7 @@
         <v>2041</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>2122</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.15">
@@ -13388,7 +13385,7 @@
         <v>1924</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.15">
@@ -13396,7 +13393,7 @@
         <v>1902</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>2106</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.15">
@@ -13404,7 +13401,7 @@
         <v>1903</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>2107</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.15">
@@ -13412,7 +13409,7 @@
         <v>1935</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>2123</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.15">
@@ -13420,7 +13417,7 @@
         <v>1935</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.15">
@@ -13428,7 +13425,7 @@
         <v>1859</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>2125</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.15">
@@ -13436,7 +13433,7 @@
         <v>1976</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>2126</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.15">
@@ -13444,7 +13441,7 @@
         <v>311</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>2127</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
@@ -13452,7 +13449,7 @@
         <v>2017</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>2128</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.15">
@@ -13460,7 +13457,7 @@
         <v>1899</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>2219</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.15">
@@ -13468,7 +13465,7 @@
         <v>1989</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>2220</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.15">
@@ -13476,7 +13473,7 @@
         <v>1919</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>2221</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.15">
@@ -13484,7 +13481,7 @@
         <v>1905</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>2222</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
@@ -13492,7 +13489,7 @@
         <v>1949</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>2223</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.15">
@@ -13500,7 +13497,7 @@
         <v>2023</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>2224</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.15">
@@ -13508,7 +13505,7 @@
         <v>1969</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>2225</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.15">
@@ -13516,7 +13513,7 @@
         <v>1996</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>2226</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.15">
@@ -13524,7 +13521,7 @@
         <v>2042</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>2227</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
@@ -13532,7 +13529,7 @@
         <v>2036</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>2228</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.15">
@@ -13540,7 +13537,7 @@
         <v>1956</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>2229</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.15">
@@ -13548,7 +13545,7 @@
         <v>2020</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>2230</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.15">
@@ -13556,7 +13553,7 @@
         <v>2034</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>2231</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.15">
@@ -13564,7 +13561,7 @@
         <v>1867</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>2232</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.15">
@@ -13572,7 +13569,7 @@
         <v>1926</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>2233</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.15">
@@ -13580,7 +13577,7 @@
         <v>1881</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>2234</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.15">
@@ -13588,7 +13585,7 @@
         <v>1980</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>2235</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.15">
@@ -13596,7 +13593,7 @@
         <v>1981</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>2236</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.15">
@@ -13604,7 +13601,7 @@
         <v>1957</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>2286</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.15">
@@ -13612,7 +13609,7 @@
         <v>1887</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>2287</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.15">
@@ -13620,7 +13617,7 @@
         <v>1861</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>2307</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.15">
@@ -13628,12 +13625,12 @@
         <v>1860</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>2308</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B124" s="4" t="s">
-        <v>2309</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.15">
@@ -13641,7 +13638,7 @@
         <v>1947</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>2310</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.15">
@@ -13649,7 +13646,7 @@
         <v>1948</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>2311</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.15">
@@ -13657,7 +13654,7 @@
         <v>2012</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>2312</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.15">
@@ -13665,7 +13662,7 @@
         <v>2013</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>2313</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.15">
@@ -13673,7 +13670,7 @@
         <v>1856</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>2314</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.15">
@@ -13681,7 +13678,7 @@
         <v>2014</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>2315</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.15">
@@ -13689,7 +13686,7 @@
         <v>1963</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>2316</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.15">
@@ -13697,7 +13694,7 @@
         <v>1854</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>2317</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.15">
@@ -13705,7 +13702,7 @@
         <v>1894</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>2318</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.15">
@@ -13713,7 +13710,7 @@
         <v>2018</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>2319</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.15">
@@ -13721,7 +13718,7 @@
         <v>1857</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.15">
@@ -13729,7 +13726,7 @@
         <v>1912</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>2321</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.15">
@@ -13737,7 +13734,7 @@
         <v>1925</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>2322</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.15">
@@ -14082,7 +14079,7 @@
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="s">
-        <v>2237</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.15">
@@ -14092,97 +14089,97 @@
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="s">
-        <v>2240</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="s">
-        <v>2241</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
-        <v>2242</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
-        <v>2243</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="s">
-        <v>2244</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
-        <v>2245</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
-        <v>2246</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
-        <v>2247</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
-        <v>2249</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
-        <v>2251</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
-        <v>2252</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
-        <v>2253</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
-        <v>2254</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
-        <v>2255</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
-        <v>2256</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
-        <v>2257</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
-        <v>2258</v>
+        <v>2253</v>
       </c>
     </row>
   </sheetData>
@@ -14213,16 +14210,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>2157</v>
+        <v>2153</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2158</v>
+        <v>2154</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2159</v>
+        <v>2155</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>2184</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -14252,13 +14249,13 @@
         <v>812</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2278</v>
+        <v>2273</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>849</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>2267</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -14285,7 +14282,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>2263</v>
+        <v>2258</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>1598</v>
@@ -14296,7 +14293,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>2262</v>
+        <v>2257</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>951</v>
@@ -14305,7 +14302,7 @@
         <v>836</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>2281</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -14326,7 +14323,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>852</v>
@@ -14334,13 +14331,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>853</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>2268</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
@@ -14435,7 +14432,7 @@
         <v>834</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>2259</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
@@ -14528,7 +14525,7 @@
         <v>872</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>2260</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.15">
@@ -14536,7 +14533,7 @@
         <v>873</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>2269</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.15">
@@ -14564,7 +14561,7 @@
         <v>827</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>2181</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.15">
@@ -14577,7 +14574,7 @@
         <v>876</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>2279</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.15">
@@ -14585,7 +14582,7 @@
         <v>877</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>2280</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.15">
@@ -14660,7 +14657,7 @@
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C67" s="4" t="s">
-        <v>2173</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.15">
@@ -14675,12 +14672,12 @@
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C70" s="4" t="s">
-        <v>2171</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C71" s="4" t="s">
-        <v>2172</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.15">
@@ -14738,7 +14735,7 @@
         <v>828</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.15">
@@ -14826,7 +14823,7 @@
         <v>907</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>2264</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.15">
@@ -14914,7 +14911,7 @@
         <v>826</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>2180</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.15">
@@ -14947,7 +14944,7 @@
         <v>833</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>2179</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="124" spans="3:4" x14ac:dyDescent="0.15">
@@ -14955,7 +14952,7 @@
         <v>926</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>2265</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="125" spans="3:4" x14ac:dyDescent="0.15">
@@ -14963,7 +14960,7 @@
         <v>927</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>2266</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="126" spans="3:4" x14ac:dyDescent="0.15">
@@ -14971,7 +14968,7 @@
         <v>835</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="127" spans="3:4" x14ac:dyDescent="0.15">
@@ -14979,7 +14976,7 @@
         <v>928</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="128" spans="3:4" x14ac:dyDescent="0.15">
@@ -14987,7 +14984,7 @@
         <v>929</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="129" spans="3:4" x14ac:dyDescent="0.15">
@@ -15010,7 +15007,7 @@
         <v>933</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>2183</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.15">
@@ -15025,15 +15022,15 @@
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C135" s="4" t="s">
-        <v>2174</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="136" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C136" s="4" t="s">
-        <v>2282</v>
+        <v>2277</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>2283</v>
+        <v>2278</v>
       </c>
     </row>
   </sheetData>
@@ -15063,16 +15060,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2160</v>
+        <v>2156</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2161</v>
+        <v>2157</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>2162</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -15499,7 +15496,7 @@
         <v>1480</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>2176</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -15631,7 +15628,7 @@
         <v>1444</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>2175</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
@@ -17196,8 +17193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D50F3D-FFC8-8A4A-AE6D-406004476759}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="178" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -17211,13 +17208,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>2163</v>
+        <v>2159</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2164</v>
+        <v>2160</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2165</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -17321,7 +17318,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>2285</v>
+        <v>2280</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1751</v>
@@ -17343,7 +17340,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>2343</v>
+        <v>2338</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>1810</v>
@@ -17354,7 +17351,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>2342</v>
+        <v>2337</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>1811</v>
@@ -17387,7 +17384,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>2325</v>
+        <v>2320</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>1798</v>
@@ -17398,7 +17395,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>2326</v>
+        <v>2321</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>1812</v>
@@ -17409,40 +17406,40 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>2327</v>
+        <v>2322</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>1789</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>2182</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>2328</v>
+        <v>2323</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>1799</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>2323</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>2329</v>
+        <v>2324</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>1748</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>2324</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>2330</v>
+        <v>2325</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>1765</v>
@@ -17450,7 +17447,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>2331</v>
+        <v>2326</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>1753</v>
@@ -17458,7 +17455,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>2341</v>
+        <v>2336</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>1764</v>
@@ -17466,7 +17463,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
-        <v>2340</v>
+        <v>2335</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>1835</v>
@@ -17474,7 +17471,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>2332</v>
+        <v>2327</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>1833</v>
@@ -17482,7 +17479,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>2333</v>
+        <v>2328</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>1778</v>
@@ -17490,7 +17487,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>2334</v>
+        <v>2329</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>1826</v>
@@ -17498,7 +17495,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>2335</v>
+        <v>2330</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>1823</v>
@@ -17506,7 +17503,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>2336</v>
+        <v>2331</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>1827</v>
@@ -17514,7 +17511,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
-        <v>2339</v>
+        <v>2334</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>1754</v>
@@ -17522,7 +17519,7 @@
     </row>
     <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>2338</v>
+        <v>2333</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>1779</v>
@@ -17530,7 +17527,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
-        <v>2337</v>
+        <v>2332</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>1800</v>
@@ -17773,102 +17770,102 @@
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B81" s="4" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B82" s="4" t="s">
-        <v>2288</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B83" s="4" t="s">
-        <v>2289</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15" x14ac:dyDescent="0.2">
       <c r="B84" s="12" t="s">
-        <v>2290</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B85" s="4" t="s">
-        <v>2291</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B86" s="4" t="s">
-        <v>2295</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B87" s="4" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B88" s="4" t="s">
-        <v>2294</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B89" s="4" t="s">
-        <v>2293</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B90" s="4" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B91" s="4" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B92" s="4" t="s">
-        <v>2298</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B93" s="4" t="s">
-        <v>2299</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="94" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B94" s="11" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B95" s="4" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B96" s="4" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B97" s="4" t="s">
-        <v>2303</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B98" s="4" t="s">
-        <v>2304</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B99" s="4" t="s">
-        <v>2305</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B100" s="4" t="s">
-        <v>2306</v>
+        <v>2301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>